<commit_message>
make it runnable for f1-f5
</commit_message>
<xml_diff>
--- a/FunctionsBounds.xlsx
+++ b/FunctionsBounds.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Metaheuristic Algorithms\Metaheur-opt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Farshid\GitHub\Metaheur-opt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -417,15 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:CB11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="BS10" sqref="BS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -456,325 +456,487 @@
       <c r="J1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1">
+        <v>6</v>
+      </c>
+      <c r="L1">
+        <v>6</v>
+      </c>
+      <c r="M1">
+        <v>7</v>
+      </c>
+      <c r="N1">
+        <v>7</v>
+      </c>
+      <c r="O1">
+        <v>8</v>
+      </c>
+      <c r="P1">
+        <v>8</v>
+      </c>
+      <c r="Q1">
+        <v>9</v>
+      </c>
+      <c r="R1">
+        <v>9</v>
+      </c>
+      <c r="S1">
+        <v>10</v>
+      </c>
+      <c r="T1">
+        <v>10</v>
+      </c>
+      <c r="U1">
+        <v>11</v>
+      </c>
+      <c r="V1">
+        <v>11</v>
+      </c>
+      <c r="W1">
+        <v>12</v>
+      </c>
+      <c r="X1">
+        <v>12</v>
+      </c>
+      <c r="Y1">
+        <v>13</v>
+      </c>
+      <c r="Z1">
+        <v>13</v>
+      </c>
+      <c r="AA1">
+        <v>14</v>
+      </c>
+      <c r="AB1">
+        <v>14</v>
+      </c>
+      <c r="AC1">
+        <v>15</v>
+      </c>
+      <c r="AD1">
+        <v>15</v>
+      </c>
+      <c r="AE1">
+        <v>16</v>
+      </c>
+      <c r="AF1">
+        <v>16</v>
+      </c>
+      <c r="AG1">
+        <v>17</v>
+      </c>
+      <c r="AH1">
+        <v>17</v>
+      </c>
+      <c r="AI1">
+        <v>18</v>
+      </c>
+      <c r="AJ1">
+        <v>18</v>
+      </c>
+      <c r="AK1">
+        <v>19</v>
+      </c>
+      <c r="AL1">
+        <v>19</v>
+      </c>
+      <c r="AM1">
+        <v>20</v>
+      </c>
+      <c r="AN1">
+        <v>20</v>
+      </c>
+      <c r="AO1">
+        <v>21</v>
+      </c>
+      <c r="AP1">
+        <v>21</v>
+      </c>
+      <c r="AQ1">
+        <v>22</v>
+      </c>
+      <c r="AR1">
+        <v>22</v>
+      </c>
+      <c r="AS1">
+        <v>23</v>
+      </c>
+      <c r="AT1">
+        <v>23</v>
+      </c>
+      <c r="AU1">
+        <v>24</v>
+      </c>
+      <c r="AV1">
+        <v>24</v>
+      </c>
+      <c r="AW1">
+        <v>25</v>
+      </c>
+      <c r="AX1">
+        <v>25</v>
+      </c>
+      <c r="AY1">
+        <v>26</v>
+      </c>
+      <c r="AZ1">
+        <v>26</v>
+      </c>
+      <c r="BA1">
+        <v>27</v>
+      </c>
+      <c r="BB1">
+        <v>27</v>
+      </c>
+      <c r="BC1">
+        <v>28</v>
+      </c>
+      <c r="BD1">
+        <v>28</v>
+      </c>
+      <c r="BE1">
+        <v>29</v>
+      </c>
+      <c r="BF1">
+        <v>29</v>
+      </c>
+      <c r="BG1">
+        <v>30</v>
+      </c>
+      <c r="BH1">
+        <v>30</v>
+      </c>
+      <c r="BI1">
+        <v>31</v>
+      </c>
+      <c r="BJ1">
+        <v>31</v>
+      </c>
+      <c r="BK1">
+        <v>32</v>
+      </c>
+      <c r="BL1">
+        <v>32</v>
+      </c>
+      <c r="BM1">
+        <v>33</v>
+      </c>
+      <c r="BN1">
+        <v>33</v>
+      </c>
+      <c r="BO1">
+        <v>34</v>
+      </c>
+      <c r="BP1">
+        <v>34</v>
+      </c>
+      <c r="BQ1">
+        <v>35</v>
+      </c>
+      <c r="BR1">
+        <v>35</v>
+      </c>
+      <c r="BS1">
+        <v>36</v>
+      </c>
+      <c r="BT1">
+        <v>36</v>
+      </c>
+      <c r="BU1">
+        <v>37</v>
+      </c>
+      <c r="BV1">
+        <v>37</v>
+      </c>
+      <c r="BW1">
+        <v>38</v>
+      </c>
+      <c r="BX1">
+        <v>38</v>
+      </c>
+      <c r="BY1">
+        <v>39</v>
+      </c>
+      <c r="BZ1">
+        <v>39</v>
+      </c>
+      <c r="CA1">
+        <v>40</v>
+      </c>
+      <c r="CB1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-100</v>
+        <v>-32</v>
       </c>
       <c r="B2">
-        <v>100</v>
-      </c>
-      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="AK2">
         <v>-30</v>
       </c>
-      <c r="D2">
+      <c r="AL2">
         <v>30</v>
       </c>
-      <c r="E2">
+      <c r="BC2">
         <v>-600</v>
       </c>
-      <c r="F2">
+      <c r="BD2">
         <v>600</v>
       </c>
-      <c r="G2">
+      <c r="BM2">
         <v>-10</v>
       </c>
-      <c r="H2">
+      <c r="BN2">
         <v>10</v>
       </c>
-      <c r="I2">
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>-32</v>
       </c>
-      <c r="J2">
+      <c r="B3">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>-100</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
+      <c r="AK3">
         <v>-30</v>
       </c>
-      <c r="D3">
+      <c r="AL3">
         <v>30</v>
       </c>
-      <c r="E3">
+      <c r="BC3">
         <v>-600</v>
       </c>
-      <c r="F3">
+      <c r="BD3">
         <v>600</v>
       </c>
-      <c r="G3">
+      <c r="BM3">
         <v>-10</v>
       </c>
-      <c r="H3">
+      <c r="BN3">
         <v>10</v>
       </c>
-      <c r="I3">
+      <c r="BU3">
+        <v>0</v>
+      </c>
+      <c r="BV3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>-32</v>
       </c>
-      <c r="J3">
+      <c r="B4">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>-100</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
+      <c r="AK4">
         <v>-30</v>
       </c>
-      <c r="D4">
+      <c r="AL4">
         <v>30</v>
       </c>
-      <c r="E4">
+      <c r="BC4">
         <v>-600</v>
       </c>
-      <c r="F4">
+      <c r="BD4">
         <v>600</v>
       </c>
-      <c r="G4">
+      <c r="BM4">
         <v>-10</v>
       </c>
-      <c r="H4">
+      <c r="BN4">
         <v>10</v>
       </c>
-      <c r="I4">
+    </row>
+    <row r="5" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>-32</v>
       </c>
-      <c r="J4">
+      <c r="B5">
         <v>32</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>-100</v>
-      </c>
-      <c r="B5">
-        <v>100</v>
-      </c>
-      <c r="C5">
+      <c r="AK5">
         <v>-30</v>
       </c>
-      <c r="D5">
+      <c r="AL5">
         <v>30</v>
       </c>
-      <c r="E5">
+      <c r="BC5">
         <v>-600</v>
       </c>
-      <c r="F5">
+      <c r="BD5">
         <v>600</v>
       </c>
-      <c r="G5">
+      <c r="BM5">
         <v>-10</v>
       </c>
-      <c r="H5">
+      <c r="BN5">
         <v>10</v>
       </c>
-      <c r="I5">
+    </row>
+    <row r="6" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>-32</v>
       </c>
-      <c r="J5">
+      <c r="B6">
         <v>32</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>-100</v>
-      </c>
-      <c r="B6">
-        <v>100</v>
-      </c>
-      <c r="C6">
+      <c r="AK6">
         <v>-30</v>
       </c>
-      <c r="D6">
+      <c r="AL6">
         <v>30</v>
       </c>
-      <c r="E6">
+      <c r="BC6">
         <v>-600</v>
       </c>
-      <c r="F6">
+      <c r="BD6">
         <v>600</v>
       </c>
-      <c r="G6">
+      <c r="BM6">
         <v>-10</v>
       </c>
-      <c r="H6">
+      <c r="BN6">
         <v>10</v>
       </c>
-      <c r="I6">
+    </row>
+    <row r="7" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>-32</v>
       </c>
-      <c r="J6">
+      <c r="B7">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>-100</v>
-      </c>
-      <c r="B7">
-        <v>100</v>
-      </c>
-      <c r="C7">
+      <c r="AK7">
         <v>-30</v>
       </c>
-      <c r="D7">
+      <c r="AL7">
         <v>30</v>
       </c>
-      <c r="E7">
+      <c r="BC7">
         <v>-600</v>
       </c>
-      <c r="F7">
+      <c r="BD7">
         <v>600</v>
       </c>
-      <c r="G7">
+      <c r="BM7">
         <v>-10</v>
       </c>
-      <c r="H7">
+      <c r="BN7">
         <v>10</v>
       </c>
-      <c r="I7">
+    </row>
+    <row r="8" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>-32</v>
       </c>
-      <c r="J7">
+      <c r="B8">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>-100</v>
-      </c>
-      <c r="B8">
-        <v>100</v>
-      </c>
-      <c r="C8">
+      <c r="AK8">
         <v>-30</v>
       </c>
-      <c r="D8">
+      <c r="AL8">
         <v>30</v>
       </c>
-      <c r="E8">
+      <c r="BC8">
         <v>-600</v>
       </c>
-      <c r="F8">
+      <c r="BD8">
         <v>600</v>
       </c>
-      <c r="G8">
+      <c r="BM8">
         <v>-10</v>
       </c>
-      <c r="H8">
+      <c r="BN8">
         <v>10</v>
       </c>
-      <c r="I8">
+    </row>
+    <row r="9" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A9">
         <v>-32</v>
       </c>
-      <c r="J8">
+      <c r="B9">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>-100</v>
-      </c>
-      <c r="B9">
-        <v>100</v>
-      </c>
-      <c r="C9">
+      <c r="AK9">
         <v>-30</v>
       </c>
-      <c r="D9">
+      <c r="AL9">
         <v>30</v>
       </c>
-      <c r="E9">
+      <c r="BC9">
         <v>-600</v>
       </c>
-      <c r="F9">
+      <c r="BD9">
         <v>600</v>
       </c>
-      <c r="G9">
+      <c r="BM9">
         <v>-10</v>
       </c>
-      <c r="H9">
+      <c r="BN9">
         <v>10</v>
       </c>
-      <c r="I9">
+    </row>
+    <row r="10" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>-32</v>
       </c>
-      <c r="J9">
+      <c r="B10">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>-100</v>
-      </c>
-      <c r="B10">
-        <v>100</v>
-      </c>
-      <c r="C10">
+      <c r="AK10">
         <v>-30</v>
       </c>
-      <c r="D10">
+      <c r="AL10">
         <v>30</v>
       </c>
-      <c r="E10">
+      <c r="BC10">
         <v>-600</v>
       </c>
-      <c r="F10">
+      <c r="BD10">
         <v>600</v>
       </c>
-      <c r="G10">
+      <c r="BM10">
         <v>-10</v>
       </c>
-      <c r="H10">
+      <c r="BN10">
         <v>10</v>
       </c>
-      <c r="I10">
+    </row>
+    <row r="11" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A11">
         <v>-32</v>
       </c>
-      <c r="J10">
+      <c r="B11">
         <v>32</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>-100</v>
-      </c>
-      <c r="B11">
-        <v>100</v>
-      </c>
-      <c r="C11">
+      <c r="AK11">
         <v>-30</v>
       </c>
-      <c r="D11">
+      <c r="AL11">
         <v>30</v>
       </c>
-      <c r="E11">
+      <c r="BC11">
         <v>-600</v>
       </c>
-      <c r="F11">
+      <c r="BD11">
         <v>600</v>
       </c>
-      <c r="G11">
+      <c r="BM11">
         <v>-10</v>
       </c>
-      <c r="H11">
+      <c r="BN11">
         <v>10</v>
-      </c>
-      <c r="I11">
-        <v>-32</v>
-      </c>
-      <c r="J11">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding new eng functions
</commit_message>
<xml_diff>
--- a/FunctionsBounds.xlsx
+++ b/FunctionsBounds.xlsx
@@ -417,15 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CB11"/>
+  <dimension ref="A1:CD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="BS10" sqref="BS10"/>
+    <sheetView tabSelected="1" topLeftCell="BN1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="BY4" sqref="BY4:BZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -666,8 +666,14 @@
       <c r="CB1">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="CC1">
+        <v>41</v>
+      </c>
+      <c r="CD1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-32</v>
       </c>
@@ -692,14 +698,32 @@
       <c r="BN2">
         <v>10</v>
       </c>
+      <c r="BS2">
+        <v>12</v>
+      </c>
+      <c r="BT2">
+        <v>60</v>
+      </c>
       <c r="BU2">
         <v>0</v>
       </c>
       <c r="BV2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="BZ2">
+        <v>12.01</v>
+      </c>
+      <c r="CC2">
+        <v>0.05</v>
+      </c>
+      <c r="CD2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-32</v>
       </c>
@@ -724,14 +748,32 @@
       <c r="BN3">
         <v>10</v>
       </c>
+      <c r="BS3">
+        <v>12</v>
+      </c>
+      <c r="BT3">
+        <v>60</v>
+      </c>
       <c r="BU3">
         <v>0</v>
       </c>
       <c r="BV3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="BY3">
+        <v>0</v>
+      </c>
+      <c r="BZ3">
+        <v>12.01</v>
+      </c>
+      <c r="CC3">
+        <v>0.25</v>
+      </c>
+      <c r="CD3">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-32</v>
       </c>
@@ -756,8 +798,26 @@
       <c r="BN4">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="BS4">
+        <v>12</v>
+      </c>
+      <c r="BT4">
+        <v>60</v>
+      </c>
+      <c r="BY4">
+        <v>0</v>
+      </c>
+      <c r="BZ4">
+        <v>12.01</v>
+      </c>
+      <c r="CC4">
+        <v>2</v>
+      </c>
+      <c r="CD4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-32</v>
       </c>
@@ -782,8 +842,20 @@
       <c r="BN5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="BS5">
+        <v>12</v>
+      </c>
+      <c r="BT5">
+        <v>60</v>
+      </c>
+      <c r="BY5">
+        <v>0</v>
+      </c>
+      <c r="BZ5">
+        <v>12.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-32</v>
       </c>
@@ -809,7 +881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-32</v>
       </c>
@@ -835,7 +907,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-32</v>
       </c>
@@ -861,7 +933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-32</v>
       </c>
@@ -887,7 +959,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-32</v>
       </c>
@@ -913,7 +985,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-32</v>
       </c>

</xml_diff>

<commit_message>
adding F8 - F23
adding F8 to F23 from Reptile 2022
</commit_message>
<xml_diff>
--- a/FunctionsBounds.xlsx
+++ b/FunctionsBounds.xlsx
@@ -417,15 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CD11"/>
+  <dimension ref="A1:DJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BR1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="BZ6" sqref="BZ6"/>
+    <sheetView tabSelected="1" topLeftCell="CV1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="DF8" sqref="DF8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:82" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -672,8 +672,104 @@
       <c r="CD1">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE1">
+        <v>108</v>
+      </c>
+      <c r="CF1">
+        <v>108</v>
+      </c>
+      <c r="CG1">
+        <v>109</v>
+      </c>
+      <c r="CH1">
+        <v>109</v>
+      </c>
+      <c r="CI1">
+        <v>110</v>
+      </c>
+      <c r="CJ1">
+        <v>110</v>
+      </c>
+      <c r="CK1">
+        <v>111</v>
+      </c>
+      <c r="CL1">
+        <v>111</v>
+      </c>
+      <c r="CM1">
+        <v>112</v>
+      </c>
+      <c r="CN1">
+        <v>112</v>
+      </c>
+      <c r="CO1">
+        <v>113</v>
+      </c>
+      <c r="CP1">
+        <v>113</v>
+      </c>
+      <c r="CQ1">
+        <v>114</v>
+      </c>
+      <c r="CR1">
+        <v>114</v>
+      </c>
+      <c r="CS1">
+        <v>115</v>
+      </c>
+      <c r="CT1">
+        <v>115</v>
+      </c>
+      <c r="CU1">
+        <v>116</v>
+      </c>
+      <c r="CV1">
+        <v>116</v>
+      </c>
+      <c r="CW1">
+        <v>117</v>
+      </c>
+      <c r="CX1">
+        <v>117</v>
+      </c>
+      <c r="CY1">
+        <v>118</v>
+      </c>
+      <c r="CZ1">
+        <v>118</v>
+      </c>
+      <c r="DA1">
+        <v>119</v>
+      </c>
+      <c r="DB1">
+        <v>119</v>
+      </c>
+      <c r="DC1">
+        <v>120</v>
+      </c>
+      <c r="DD1">
+        <v>120</v>
+      </c>
+      <c r="DE1">
+        <v>121</v>
+      </c>
+      <c r="DF1">
+        <v>121</v>
+      </c>
+      <c r="DG1">
+        <v>122</v>
+      </c>
+      <c r="DH1">
+        <v>122</v>
+      </c>
+      <c r="DI1">
+        <v>123</v>
+      </c>
+      <c r="DJ1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-32</v>
       </c>
@@ -740,8 +836,104 @@
       <c r="CD2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE2">
+        <v>-500</v>
+      </c>
+      <c r="CF2">
+        <v>500</v>
+      </c>
+      <c r="CG2">
+        <v>-5.12</v>
+      </c>
+      <c r="CH2">
+        <v>5.12</v>
+      </c>
+      <c r="CI2">
+        <v>-32</v>
+      </c>
+      <c r="CJ2">
+        <v>32</v>
+      </c>
+      <c r="CK2">
+        <v>-600</v>
+      </c>
+      <c r="CL2">
+        <v>600</v>
+      </c>
+      <c r="CM2">
+        <v>-50</v>
+      </c>
+      <c r="CN2">
+        <v>50</v>
+      </c>
+      <c r="CO2">
+        <v>-50</v>
+      </c>
+      <c r="CP2">
+        <v>50</v>
+      </c>
+      <c r="CQ2">
+        <v>-65</v>
+      </c>
+      <c r="CR2">
+        <v>65</v>
+      </c>
+      <c r="CS2">
+        <v>-5</v>
+      </c>
+      <c r="CT2">
+        <v>5</v>
+      </c>
+      <c r="CU2">
+        <v>-5</v>
+      </c>
+      <c r="CV2">
+        <v>5</v>
+      </c>
+      <c r="CW2">
+        <v>-5</v>
+      </c>
+      <c r="CX2">
+        <v>5</v>
+      </c>
+      <c r="CY2">
+        <v>-2</v>
+      </c>
+      <c r="CZ2">
+        <v>2</v>
+      </c>
+      <c r="DA2">
+        <v>-1</v>
+      </c>
+      <c r="DB2">
+        <v>1</v>
+      </c>
+      <c r="DC2">
+        <v>0</v>
+      </c>
+      <c r="DD2">
+        <v>1</v>
+      </c>
+      <c r="DE2">
+        <v>0</v>
+      </c>
+      <c r="DF2">
+        <v>1</v>
+      </c>
+      <c r="DG2">
+        <v>0</v>
+      </c>
+      <c r="DH2">
+        <v>1</v>
+      </c>
+      <c r="DI2">
+        <v>0</v>
+      </c>
+      <c r="DJ2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-32</v>
       </c>
@@ -808,8 +1000,104 @@
       <c r="CD3">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE3">
+        <v>-500</v>
+      </c>
+      <c r="CF3">
+        <v>500</v>
+      </c>
+      <c r="CG3">
+        <v>-5.12</v>
+      </c>
+      <c r="CH3">
+        <v>5.12</v>
+      </c>
+      <c r="CI3">
+        <v>-32</v>
+      </c>
+      <c r="CJ3">
+        <v>32</v>
+      </c>
+      <c r="CK3">
+        <v>-600</v>
+      </c>
+      <c r="CL3">
+        <v>600</v>
+      </c>
+      <c r="CM3">
+        <v>-50</v>
+      </c>
+      <c r="CN3">
+        <v>50</v>
+      </c>
+      <c r="CO3">
+        <v>-50</v>
+      </c>
+      <c r="CP3">
+        <v>50</v>
+      </c>
+      <c r="CQ3">
+        <v>-65</v>
+      </c>
+      <c r="CR3">
+        <v>65</v>
+      </c>
+      <c r="CS3">
+        <v>-5</v>
+      </c>
+      <c r="CT3">
+        <v>5</v>
+      </c>
+      <c r="CU3">
+        <v>-5</v>
+      </c>
+      <c r="CV3">
+        <v>5</v>
+      </c>
+      <c r="CW3">
+        <v>-5</v>
+      </c>
+      <c r="CX3">
+        <v>5</v>
+      </c>
+      <c r="CY3">
+        <v>-2</v>
+      </c>
+      <c r="CZ3">
+        <v>2</v>
+      </c>
+      <c r="DA3">
+        <v>-1</v>
+      </c>
+      <c r="DB3">
+        <v>1</v>
+      </c>
+      <c r="DC3">
+        <v>0</v>
+      </c>
+      <c r="DD3">
+        <v>1</v>
+      </c>
+      <c r="DE3">
+        <v>0</v>
+      </c>
+      <c r="DF3">
+        <v>1</v>
+      </c>
+      <c r="DG3">
+        <v>0</v>
+      </c>
+      <c r="DH3">
+        <v>1</v>
+      </c>
+      <c r="DI3">
+        <v>0</v>
+      </c>
+      <c r="DJ3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-32</v>
       </c>
@@ -870,8 +1158,80 @@
       <c r="CD4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE4">
+        <v>-500</v>
+      </c>
+      <c r="CF4">
+        <v>500</v>
+      </c>
+      <c r="CG4">
+        <v>-5.12</v>
+      </c>
+      <c r="CH4">
+        <v>5.12</v>
+      </c>
+      <c r="CI4">
+        <v>-32</v>
+      </c>
+      <c r="CJ4">
+        <v>32</v>
+      </c>
+      <c r="CK4">
+        <v>-600</v>
+      </c>
+      <c r="CL4">
+        <v>600</v>
+      </c>
+      <c r="CM4">
+        <v>-50</v>
+      </c>
+      <c r="CN4">
+        <v>50</v>
+      </c>
+      <c r="CO4">
+        <v>-50</v>
+      </c>
+      <c r="CP4">
+        <v>50</v>
+      </c>
+      <c r="CS4">
+        <v>-5</v>
+      </c>
+      <c r="CT4">
+        <v>5</v>
+      </c>
+      <c r="DA4">
+        <v>-1</v>
+      </c>
+      <c r="DB4">
+        <v>1</v>
+      </c>
+      <c r="DC4">
+        <v>0</v>
+      </c>
+      <c r="DD4">
+        <v>1</v>
+      </c>
+      <c r="DE4">
+        <v>0</v>
+      </c>
+      <c r="DF4">
+        <v>1</v>
+      </c>
+      <c r="DG4">
+        <v>0</v>
+      </c>
+      <c r="DH4">
+        <v>1</v>
+      </c>
+      <c r="DI4">
+        <v>0</v>
+      </c>
+      <c r="DJ4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-32</v>
       </c>
@@ -926,8 +1286,74 @@
       <c r="BZ5">
         <v>10000</v>
       </c>
-    </row>
-    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE5">
+        <v>-500</v>
+      </c>
+      <c r="CF5">
+        <v>500</v>
+      </c>
+      <c r="CG5">
+        <v>-5.12</v>
+      </c>
+      <c r="CH5">
+        <v>5.12</v>
+      </c>
+      <c r="CI5">
+        <v>-32</v>
+      </c>
+      <c r="CJ5">
+        <v>32</v>
+      </c>
+      <c r="CK5">
+        <v>-600</v>
+      </c>
+      <c r="CL5">
+        <v>600</v>
+      </c>
+      <c r="CM5">
+        <v>-50</v>
+      </c>
+      <c r="CN5">
+        <v>50</v>
+      </c>
+      <c r="CO5">
+        <v>-50</v>
+      </c>
+      <c r="CP5">
+        <v>50</v>
+      </c>
+      <c r="CS5">
+        <v>-5</v>
+      </c>
+      <c r="CT5">
+        <v>5</v>
+      </c>
+      <c r="DC5">
+        <v>0</v>
+      </c>
+      <c r="DD5">
+        <v>1</v>
+      </c>
+      <c r="DE5">
+        <v>0</v>
+      </c>
+      <c r="DF5">
+        <v>1</v>
+      </c>
+      <c r="DG5">
+        <v>0</v>
+      </c>
+      <c r="DH5">
+        <v>1</v>
+      </c>
+      <c r="DI5">
+        <v>0</v>
+      </c>
+      <c r="DJ5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-32</v>
       </c>
@@ -958,8 +1384,50 @@
       <c r="BN6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE6">
+        <v>-500</v>
+      </c>
+      <c r="CF6">
+        <v>500</v>
+      </c>
+      <c r="CG6">
+        <v>-5.12</v>
+      </c>
+      <c r="CH6">
+        <v>5.12</v>
+      </c>
+      <c r="CI6">
+        <v>-32</v>
+      </c>
+      <c r="CJ6">
+        <v>32</v>
+      </c>
+      <c r="CK6">
+        <v>-600</v>
+      </c>
+      <c r="CL6">
+        <v>600</v>
+      </c>
+      <c r="CM6">
+        <v>-50</v>
+      </c>
+      <c r="CN6">
+        <v>50</v>
+      </c>
+      <c r="CO6">
+        <v>-50</v>
+      </c>
+      <c r="CP6">
+        <v>50</v>
+      </c>
+      <c r="DC6">
+        <v>0</v>
+      </c>
+      <c r="DD6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-32</v>
       </c>
@@ -990,8 +1458,50 @@
       <c r="BN7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE7">
+        <v>-500</v>
+      </c>
+      <c r="CF7">
+        <v>500</v>
+      </c>
+      <c r="CG7">
+        <v>-5.12</v>
+      </c>
+      <c r="CH7">
+        <v>5.12</v>
+      </c>
+      <c r="CI7">
+        <v>-32</v>
+      </c>
+      <c r="CJ7">
+        <v>32</v>
+      </c>
+      <c r="CK7">
+        <v>-600</v>
+      </c>
+      <c r="CL7">
+        <v>600</v>
+      </c>
+      <c r="CM7">
+        <v>-50</v>
+      </c>
+      <c r="CN7">
+        <v>50</v>
+      </c>
+      <c r="CO7">
+        <v>-50</v>
+      </c>
+      <c r="CP7">
+        <v>50</v>
+      </c>
+      <c r="DC7">
+        <v>0</v>
+      </c>
+      <c r="DD7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-32</v>
       </c>
@@ -1022,8 +1532,44 @@
       <c r="BN8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE8">
+        <v>-500</v>
+      </c>
+      <c r="CF8">
+        <v>500</v>
+      </c>
+      <c r="CG8">
+        <v>-5.12</v>
+      </c>
+      <c r="CH8">
+        <v>5.12</v>
+      </c>
+      <c r="CI8">
+        <v>-32</v>
+      </c>
+      <c r="CJ8">
+        <v>32</v>
+      </c>
+      <c r="CK8">
+        <v>-600</v>
+      </c>
+      <c r="CL8">
+        <v>600</v>
+      </c>
+      <c r="CM8">
+        <v>-50</v>
+      </c>
+      <c r="CN8">
+        <v>50</v>
+      </c>
+      <c r="CO8">
+        <v>-50</v>
+      </c>
+      <c r="CP8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-32</v>
       </c>
@@ -1054,8 +1600,44 @@
       <c r="BN9">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE9">
+        <v>-500</v>
+      </c>
+      <c r="CF9">
+        <v>500</v>
+      </c>
+      <c r="CG9">
+        <v>-5.12</v>
+      </c>
+      <c r="CH9">
+        <v>5.12</v>
+      </c>
+      <c r="CI9">
+        <v>-32</v>
+      </c>
+      <c r="CJ9">
+        <v>32</v>
+      </c>
+      <c r="CK9">
+        <v>-600</v>
+      </c>
+      <c r="CL9">
+        <v>600</v>
+      </c>
+      <c r="CM9">
+        <v>-50</v>
+      </c>
+      <c r="CN9">
+        <v>50</v>
+      </c>
+      <c r="CO9">
+        <v>-50</v>
+      </c>
+      <c r="CP9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-32</v>
       </c>
@@ -1086,8 +1668,44 @@
       <c r="BN10">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
+      <c r="CE10">
+        <v>-500</v>
+      </c>
+      <c r="CF10">
+        <v>500</v>
+      </c>
+      <c r="CG10">
+        <v>-5.12</v>
+      </c>
+      <c r="CH10">
+        <v>5.12</v>
+      </c>
+      <c r="CI10">
+        <v>-32</v>
+      </c>
+      <c r="CJ10">
+        <v>32</v>
+      </c>
+      <c r="CK10">
+        <v>-600</v>
+      </c>
+      <c r="CL10">
+        <v>600</v>
+      </c>
+      <c r="CM10">
+        <v>-50</v>
+      </c>
+      <c r="CN10">
+        <v>50</v>
+      </c>
+      <c r="CO10">
+        <v>-50</v>
+      </c>
+      <c r="CP10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:114" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-32</v>
       </c>
@@ -1117,6 +1735,3462 @@
       </c>
       <c r="BN11">
         <v>10</v>
+      </c>
+      <c r="CE11">
+        <v>-500</v>
+      </c>
+      <c r="CF11">
+        <v>500</v>
+      </c>
+      <c r="CG11">
+        <v>-5.12</v>
+      </c>
+      <c r="CH11">
+        <v>5.12</v>
+      </c>
+      <c r="CI11">
+        <v>-32</v>
+      </c>
+      <c r="CJ11">
+        <v>32</v>
+      </c>
+      <c r="CK11">
+        <v>-600</v>
+      </c>
+      <c r="CL11">
+        <v>600</v>
+      </c>
+      <c r="CM11">
+        <v>-50</v>
+      </c>
+      <c r="CN11">
+        <v>50</v>
+      </c>
+      <c r="CO11">
+        <v>-50</v>
+      </c>
+      <c r="CP11">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:114" x14ac:dyDescent="0.25">
+      <c r="CE12">
+        <v>-500</v>
+      </c>
+      <c r="CF12">
+        <v>500</v>
+      </c>
+      <c r="CG12">
+        <v>-5.12</v>
+      </c>
+      <c r="CH12">
+        <v>5.12</v>
+      </c>
+      <c r="CI12">
+        <v>-32</v>
+      </c>
+      <c r="CJ12">
+        <v>32</v>
+      </c>
+      <c r="CK12">
+        <v>-600</v>
+      </c>
+      <c r="CL12">
+        <v>600</v>
+      </c>
+      <c r="CM12">
+        <v>-50</v>
+      </c>
+      <c r="CN12">
+        <v>50</v>
+      </c>
+      <c r="CO12">
+        <v>-50</v>
+      </c>
+      <c r="CP12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:114" x14ac:dyDescent="0.25">
+      <c r="CE13">
+        <v>-500</v>
+      </c>
+      <c r="CF13">
+        <v>500</v>
+      </c>
+      <c r="CG13">
+        <v>-5.12</v>
+      </c>
+      <c r="CH13">
+        <v>5.12</v>
+      </c>
+      <c r="CI13">
+        <v>-32</v>
+      </c>
+      <c r="CJ13">
+        <v>32</v>
+      </c>
+      <c r="CK13">
+        <v>-600</v>
+      </c>
+      <c r="CL13">
+        <v>600</v>
+      </c>
+      <c r="CM13">
+        <v>-50</v>
+      </c>
+      <c r="CN13">
+        <v>50</v>
+      </c>
+      <c r="CO13">
+        <v>-50</v>
+      </c>
+      <c r="CP13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:114" x14ac:dyDescent="0.25">
+      <c r="CE14">
+        <v>-500</v>
+      </c>
+      <c r="CF14">
+        <v>500</v>
+      </c>
+      <c r="CG14">
+        <v>-5.12</v>
+      </c>
+      <c r="CH14">
+        <v>5.12</v>
+      </c>
+      <c r="CI14">
+        <v>-32</v>
+      </c>
+      <c r="CJ14">
+        <v>32</v>
+      </c>
+      <c r="CK14">
+        <v>-600</v>
+      </c>
+      <c r="CL14">
+        <v>600</v>
+      </c>
+      <c r="CM14">
+        <v>-50</v>
+      </c>
+      <c r="CN14">
+        <v>50</v>
+      </c>
+      <c r="CO14">
+        <v>-50</v>
+      </c>
+      <c r="CP14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:114" x14ac:dyDescent="0.25">
+      <c r="CE15">
+        <v>-500</v>
+      </c>
+      <c r="CF15">
+        <v>500</v>
+      </c>
+      <c r="CG15">
+        <v>-5.12</v>
+      </c>
+      <c r="CH15">
+        <v>5.12</v>
+      </c>
+      <c r="CI15">
+        <v>-32</v>
+      </c>
+      <c r="CJ15">
+        <v>32</v>
+      </c>
+      <c r="CK15">
+        <v>-600</v>
+      </c>
+      <c r="CL15">
+        <v>600</v>
+      </c>
+      <c r="CM15">
+        <v>-50</v>
+      </c>
+      <c r="CN15">
+        <v>50</v>
+      </c>
+      <c r="CO15">
+        <v>-50</v>
+      </c>
+      <c r="CP15">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:114" x14ac:dyDescent="0.25">
+      <c r="CE16">
+        <v>-500</v>
+      </c>
+      <c r="CF16">
+        <v>500</v>
+      </c>
+      <c r="CG16">
+        <v>-5.12</v>
+      </c>
+      <c r="CH16">
+        <v>5.12</v>
+      </c>
+      <c r="CI16">
+        <v>-32</v>
+      </c>
+      <c r="CJ16">
+        <v>32</v>
+      </c>
+      <c r="CK16">
+        <v>-600</v>
+      </c>
+      <c r="CL16">
+        <v>600</v>
+      </c>
+      <c r="CM16">
+        <v>-50</v>
+      </c>
+      <c r="CN16">
+        <v>50</v>
+      </c>
+      <c r="CO16">
+        <v>-50</v>
+      </c>
+      <c r="CP16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE17">
+        <v>-500</v>
+      </c>
+      <c r="CF17">
+        <v>500</v>
+      </c>
+      <c r="CG17">
+        <v>-5.12</v>
+      </c>
+      <c r="CH17">
+        <v>5.12</v>
+      </c>
+      <c r="CI17">
+        <v>-32</v>
+      </c>
+      <c r="CJ17">
+        <v>32</v>
+      </c>
+      <c r="CK17">
+        <v>-600</v>
+      </c>
+      <c r="CL17">
+        <v>600</v>
+      </c>
+      <c r="CM17">
+        <v>-50</v>
+      </c>
+      <c r="CN17">
+        <v>50</v>
+      </c>
+      <c r="CO17">
+        <v>-50</v>
+      </c>
+      <c r="CP17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE18">
+        <v>-500</v>
+      </c>
+      <c r="CF18">
+        <v>500</v>
+      </c>
+      <c r="CG18">
+        <v>-5.12</v>
+      </c>
+      <c r="CH18">
+        <v>5.12</v>
+      </c>
+      <c r="CI18">
+        <v>-32</v>
+      </c>
+      <c r="CJ18">
+        <v>32</v>
+      </c>
+      <c r="CK18">
+        <v>-600</v>
+      </c>
+      <c r="CL18">
+        <v>600</v>
+      </c>
+      <c r="CM18">
+        <v>-50</v>
+      </c>
+      <c r="CN18">
+        <v>50</v>
+      </c>
+      <c r="CO18">
+        <v>-50</v>
+      </c>
+      <c r="CP18">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE19">
+        <v>-500</v>
+      </c>
+      <c r="CF19">
+        <v>500</v>
+      </c>
+      <c r="CG19">
+        <v>-5.12</v>
+      </c>
+      <c r="CH19">
+        <v>5.12</v>
+      </c>
+      <c r="CI19">
+        <v>-32</v>
+      </c>
+      <c r="CJ19">
+        <v>32</v>
+      </c>
+      <c r="CK19">
+        <v>-600</v>
+      </c>
+      <c r="CL19">
+        <v>600</v>
+      </c>
+      <c r="CM19">
+        <v>-50</v>
+      </c>
+      <c r="CN19">
+        <v>50</v>
+      </c>
+      <c r="CO19">
+        <v>-50</v>
+      </c>
+      <c r="CP19">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE20">
+        <v>-500</v>
+      </c>
+      <c r="CF20">
+        <v>500</v>
+      </c>
+      <c r="CG20">
+        <v>-5.12</v>
+      </c>
+      <c r="CH20">
+        <v>5.12</v>
+      </c>
+      <c r="CI20">
+        <v>-32</v>
+      </c>
+      <c r="CJ20">
+        <v>32</v>
+      </c>
+      <c r="CK20">
+        <v>-600</v>
+      </c>
+      <c r="CL20">
+        <v>600</v>
+      </c>
+      <c r="CM20">
+        <v>-50</v>
+      </c>
+      <c r="CN20">
+        <v>50</v>
+      </c>
+      <c r="CO20">
+        <v>-50</v>
+      </c>
+      <c r="CP20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE21">
+        <v>-500</v>
+      </c>
+      <c r="CF21">
+        <v>500</v>
+      </c>
+      <c r="CG21">
+        <v>-5.12</v>
+      </c>
+      <c r="CH21">
+        <v>5.12</v>
+      </c>
+      <c r="CI21">
+        <v>-32</v>
+      </c>
+      <c r="CJ21">
+        <v>32</v>
+      </c>
+      <c r="CK21">
+        <v>-600</v>
+      </c>
+      <c r="CL21">
+        <v>600</v>
+      </c>
+      <c r="CM21">
+        <v>-50</v>
+      </c>
+      <c r="CN21">
+        <v>50</v>
+      </c>
+      <c r="CO21">
+        <v>-50</v>
+      </c>
+      <c r="CP21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE22">
+        <v>-500</v>
+      </c>
+      <c r="CF22">
+        <v>500</v>
+      </c>
+      <c r="CG22">
+        <v>-5.12</v>
+      </c>
+      <c r="CH22">
+        <v>5.12</v>
+      </c>
+      <c r="CI22">
+        <v>-32</v>
+      </c>
+      <c r="CJ22">
+        <v>32</v>
+      </c>
+      <c r="CK22">
+        <v>-600</v>
+      </c>
+      <c r="CL22">
+        <v>600</v>
+      </c>
+      <c r="CM22">
+        <v>-50</v>
+      </c>
+      <c r="CN22">
+        <v>50</v>
+      </c>
+      <c r="CO22">
+        <v>-50</v>
+      </c>
+      <c r="CP22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE23">
+        <v>-500</v>
+      </c>
+      <c r="CF23">
+        <v>500</v>
+      </c>
+      <c r="CG23">
+        <v>-5.12</v>
+      </c>
+      <c r="CH23">
+        <v>5.12</v>
+      </c>
+      <c r="CI23">
+        <v>-32</v>
+      </c>
+      <c r="CJ23">
+        <v>32</v>
+      </c>
+      <c r="CK23">
+        <v>-600</v>
+      </c>
+      <c r="CL23">
+        <v>600</v>
+      </c>
+      <c r="CM23">
+        <v>-50</v>
+      </c>
+      <c r="CN23">
+        <v>50</v>
+      </c>
+      <c r="CO23">
+        <v>-50</v>
+      </c>
+      <c r="CP23">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE24">
+        <v>-500</v>
+      </c>
+      <c r="CF24">
+        <v>500</v>
+      </c>
+      <c r="CG24">
+        <v>-5.12</v>
+      </c>
+      <c r="CH24">
+        <v>5.12</v>
+      </c>
+      <c r="CI24">
+        <v>-32</v>
+      </c>
+      <c r="CJ24">
+        <v>32</v>
+      </c>
+      <c r="CK24">
+        <v>-600</v>
+      </c>
+      <c r="CL24">
+        <v>600</v>
+      </c>
+      <c r="CM24">
+        <v>-50</v>
+      </c>
+      <c r="CN24">
+        <v>50</v>
+      </c>
+      <c r="CO24">
+        <v>-50</v>
+      </c>
+      <c r="CP24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE25">
+        <v>-500</v>
+      </c>
+      <c r="CF25">
+        <v>500</v>
+      </c>
+      <c r="CG25">
+        <v>-5.12</v>
+      </c>
+      <c r="CH25">
+        <v>5.12</v>
+      </c>
+      <c r="CI25">
+        <v>-32</v>
+      </c>
+      <c r="CJ25">
+        <v>32</v>
+      </c>
+      <c r="CK25">
+        <v>-600</v>
+      </c>
+      <c r="CL25">
+        <v>600</v>
+      </c>
+      <c r="CM25">
+        <v>-50</v>
+      </c>
+      <c r="CN25">
+        <v>50</v>
+      </c>
+      <c r="CO25">
+        <v>-50</v>
+      </c>
+      <c r="CP25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE26">
+        <v>-500</v>
+      </c>
+      <c r="CF26">
+        <v>500</v>
+      </c>
+      <c r="CG26">
+        <v>-5.12</v>
+      </c>
+      <c r="CH26">
+        <v>5.12</v>
+      </c>
+      <c r="CI26">
+        <v>-32</v>
+      </c>
+      <c r="CJ26">
+        <v>32</v>
+      </c>
+      <c r="CK26">
+        <v>-600</v>
+      </c>
+      <c r="CL26">
+        <v>600</v>
+      </c>
+      <c r="CM26">
+        <v>-50</v>
+      </c>
+      <c r="CN26">
+        <v>50</v>
+      </c>
+      <c r="CO26">
+        <v>-50</v>
+      </c>
+      <c r="CP26">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE27">
+        <v>-500</v>
+      </c>
+      <c r="CF27">
+        <v>500</v>
+      </c>
+      <c r="CG27">
+        <v>-5.12</v>
+      </c>
+      <c r="CH27">
+        <v>5.12</v>
+      </c>
+      <c r="CI27">
+        <v>-32</v>
+      </c>
+      <c r="CJ27">
+        <v>32</v>
+      </c>
+      <c r="CK27">
+        <v>-600</v>
+      </c>
+      <c r="CL27">
+        <v>600</v>
+      </c>
+      <c r="CM27">
+        <v>-50</v>
+      </c>
+      <c r="CN27">
+        <v>50</v>
+      </c>
+      <c r="CO27">
+        <v>-50</v>
+      </c>
+      <c r="CP27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE28">
+        <v>-500</v>
+      </c>
+      <c r="CF28">
+        <v>500</v>
+      </c>
+      <c r="CG28">
+        <v>-5.12</v>
+      </c>
+      <c r="CH28">
+        <v>5.12</v>
+      </c>
+      <c r="CI28">
+        <v>-32</v>
+      </c>
+      <c r="CJ28">
+        <v>32</v>
+      </c>
+      <c r="CK28">
+        <v>-600</v>
+      </c>
+      <c r="CL28">
+        <v>600</v>
+      </c>
+      <c r="CM28">
+        <v>-50</v>
+      </c>
+      <c r="CN28">
+        <v>50</v>
+      </c>
+      <c r="CO28">
+        <v>-50</v>
+      </c>
+      <c r="CP28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE29">
+        <v>-500</v>
+      </c>
+      <c r="CF29">
+        <v>500</v>
+      </c>
+      <c r="CG29">
+        <v>-5.12</v>
+      </c>
+      <c r="CH29">
+        <v>5.12</v>
+      </c>
+      <c r="CI29">
+        <v>-32</v>
+      </c>
+      <c r="CJ29">
+        <v>32</v>
+      </c>
+      <c r="CK29">
+        <v>-600</v>
+      </c>
+      <c r="CL29">
+        <v>600</v>
+      </c>
+      <c r="CM29">
+        <v>-50</v>
+      </c>
+      <c r="CN29">
+        <v>50</v>
+      </c>
+      <c r="CO29">
+        <v>-50</v>
+      </c>
+      <c r="CP29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE30">
+        <v>-500</v>
+      </c>
+      <c r="CF30">
+        <v>500</v>
+      </c>
+      <c r="CG30">
+        <v>-5.12</v>
+      </c>
+      <c r="CH30">
+        <v>5.12</v>
+      </c>
+      <c r="CI30">
+        <v>-32</v>
+      </c>
+      <c r="CJ30">
+        <v>32</v>
+      </c>
+      <c r="CK30">
+        <v>-600</v>
+      </c>
+      <c r="CL30">
+        <v>600</v>
+      </c>
+      <c r="CM30">
+        <v>-50</v>
+      </c>
+      <c r="CN30">
+        <v>50</v>
+      </c>
+      <c r="CO30">
+        <v>-50</v>
+      </c>
+      <c r="CP30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE31">
+        <v>-500</v>
+      </c>
+      <c r="CF31">
+        <v>500</v>
+      </c>
+      <c r="CG31">
+        <v>-5.12</v>
+      </c>
+      <c r="CH31">
+        <v>5.12</v>
+      </c>
+      <c r="CI31">
+        <v>-32</v>
+      </c>
+      <c r="CJ31">
+        <v>32</v>
+      </c>
+      <c r="CK31">
+        <v>-600</v>
+      </c>
+      <c r="CL31">
+        <v>600</v>
+      </c>
+      <c r="CM31">
+        <v>-50</v>
+      </c>
+      <c r="CN31">
+        <v>50</v>
+      </c>
+      <c r="CO31">
+        <v>-50</v>
+      </c>
+      <c r="CP31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE32">
+        <v>-500</v>
+      </c>
+      <c r="CF32">
+        <v>500</v>
+      </c>
+      <c r="CG32">
+        <v>-5.12</v>
+      </c>
+      <c r="CH32">
+        <v>5.12</v>
+      </c>
+      <c r="CI32">
+        <v>-32</v>
+      </c>
+      <c r="CJ32">
+        <v>32</v>
+      </c>
+      <c r="CK32">
+        <v>-600</v>
+      </c>
+      <c r="CL32">
+        <v>600</v>
+      </c>
+      <c r="CM32">
+        <v>-50</v>
+      </c>
+      <c r="CN32">
+        <v>50</v>
+      </c>
+      <c r="CO32">
+        <v>-50</v>
+      </c>
+      <c r="CP32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE33">
+        <v>-500</v>
+      </c>
+      <c r="CF33">
+        <v>500</v>
+      </c>
+      <c r="CG33">
+        <v>-5.12</v>
+      </c>
+      <c r="CH33">
+        <v>5.12</v>
+      </c>
+      <c r="CI33">
+        <v>-32</v>
+      </c>
+      <c r="CJ33">
+        <v>32</v>
+      </c>
+      <c r="CK33">
+        <v>-600</v>
+      </c>
+      <c r="CL33">
+        <v>600</v>
+      </c>
+      <c r="CM33">
+        <v>-50</v>
+      </c>
+      <c r="CN33">
+        <v>50</v>
+      </c>
+      <c r="CO33">
+        <v>-50</v>
+      </c>
+      <c r="CP33">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE34">
+        <v>-500</v>
+      </c>
+      <c r="CF34">
+        <v>500</v>
+      </c>
+      <c r="CG34">
+        <v>-5.12</v>
+      </c>
+      <c r="CH34">
+        <v>5.12</v>
+      </c>
+      <c r="CI34">
+        <v>-32</v>
+      </c>
+      <c r="CJ34">
+        <v>32</v>
+      </c>
+      <c r="CK34">
+        <v>-600</v>
+      </c>
+      <c r="CL34">
+        <v>600</v>
+      </c>
+      <c r="CM34">
+        <v>-50</v>
+      </c>
+      <c r="CN34">
+        <v>50</v>
+      </c>
+      <c r="CO34">
+        <v>-50</v>
+      </c>
+      <c r="CP34">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE35">
+        <v>-500</v>
+      </c>
+      <c r="CF35">
+        <v>500</v>
+      </c>
+      <c r="CG35">
+        <v>-5.12</v>
+      </c>
+      <c r="CH35">
+        <v>5.12</v>
+      </c>
+      <c r="CI35">
+        <v>-32</v>
+      </c>
+      <c r="CJ35">
+        <v>32</v>
+      </c>
+      <c r="CK35">
+        <v>-600</v>
+      </c>
+      <c r="CL35">
+        <v>600</v>
+      </c>
+      <c r="CM35">
+        <v>-50</v>
+      </c>
+      <c r="CN35">
+        <v>50</v>
+      </c>
+      <c r="CO35">
+        <v>-50</v>
+      </c>
+      <c r="CP35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE36">
+        <v>-500</v>
+      </c>
+      <c r="CF36">
+        <v>500</v>
+      </c>
+      <c r="CG36">
+        <v>-5.12</v>
+      </c>
+      <c r="CH36">
+        <v>5.12</v>
+      </c>
+      <c r="CI36">
+        <v>-32</v>
+      </c>
+      <c r="CJ36">
+        <v>32</v>
+      </c>
+      <c r="CK36">
+        <v>-600</v>
+      </c>
+      <c r="CL36">
+        <v>600</v>
+      </c>
+      <c r="CM36">
+        <v>-50</v>
+      </c>
+      <c r="CN36">
+        <v>50</v>
+      </c>
+      <c r="CO36">
+        <v>-50</v>
+      </c>
+      <c r="CP36">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE37">
+        <v>-500</v>
+      </c>
+      <c r="CF37">
+        <v>500</v>
+      </c>
+      <c r="CG37">
+        <v>-5.12</v>
+      </c>
+      <c r="CH37">
+        <v>5.12</v>
+      </c>
+      <c r="CI37">
+        <v>-32</v>
+      </c>
+      <c r="CJ37">
+        <v>32</v>
+      </c>
+      <c r="CK37">
+        <v>-600</v>
+      </c>
+      <c r="CL37">
+        <v>600</v>
+      </c>
+      <c r="CM37">
+        <v>-50</v>
+      </c>
+      <c r="CN37">
+        <v>50</v>
+      </c>
+      <c r="CO37">
+        <v>-50</v>
+      </c>
+      <c r="CP37">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE38">
+        <v>-500</v>
+      </c>
+      <c r="CF38">
+        <v>500</v>
+      </c>
+      <c r="CG38">
+        <v>-5.12</v>
+      </c>
+      <c r="CH38">
+        <v>5.12</v>
+      </c>
+      <c r="CI38">
+        <v>-32</v>
+      </c>
+      <c r="CJ38">
+        <v>32</v>
+      </c>
+      <c r="CK38">
+        <v>-600</v>
+      </c>
+      <c r="CL38">
+        <v>600</v>
+      </c>
+      <c r="CM38">
+        <v>-50</v>
+      </c>
+      <c r="CN38">
+        <v>50</v>
+      </c>
+      <c r="CO38">
+        <v>-50</v>
+      </c>
+      <c r="CP38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE39">
+        <v>-500</v>
+      </c>
+      <c r="CF39">
+        <v>500</v>
+      </c>
+      <c r="CG39">
+        <v>-5.12</v>
+      </c>
+      <c r="CH39">
+        <v>5.12</v>
+      </c>
+      <c r="CI39">
+        <v>-32</v>
+      </c>
+      <c r="CJ39">
+        <v>32</v>
+      </c>
+      <c r="CK39">
+        <v>-600</v>
+      </c>
+      <c r="CL39">
+        <v>600</v>
+      </c>
+      <c r="CM39">
+        <v>-50</v>
+      </c>
+      <c r="CN39">
+        <v>50</v>
+      </c>
+      <c r="CO39">
+        <v>-50</v>
+      </c>
+      <c r="CP39">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE40">
+        <v>-500</v>
+      </c>
+      <c r="CF40">
+        <v>500</v>
+      </c>
+      <c r="CG40">
+        <v>-5.12</v>
+      </c>
+      <c r="CH40">
+        <v>5.12</v>
+      </c>
+      <c r="CI40">
+        <v>-32</v>
+      </c>
+      <c r="CJ40">
+        <v>32</v>
+      </c>
+      <c r="CK40">
+        <v>-600</v>
+      </c>
+      <c r="CL40">
+        <v>600</v>
+      </c>
+      <c r="CM40">
+        <v>-50</v>
+      </c>
+      <c r="CN40">
+        <v>50</v>
+      </c>
+      <c r="CO40">
+        <v>-50</v>
+      </c>
+      <c r="CP40">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE41">
+        <v>-500</v>
+      </c>
+      <c r="CF41">
+        <v>500</v>
+      </c>
+      <c r="CG41">
+        <v>-5.12</v>
+      </c>
+      <c r="CH41">
+        <v>5.12</v>
+      </c>
+      <c r="CI41">
+        <v>-32</v>
+      </c>
+      <c r="CJ41">
+        <v>32</v>
+      </c>
+      <c r="CK41">
+        <v>-600</v>
+      </c>
+      <c r="CL41">
+        <v>600</v>
+      </c>
+      <c r="CM41">
+        <v>-50</v>
+      </c>
+      <c r="CN41">
+        <v>50</v>
+      </c>
+      <c r="CO41">
+        <v>-50</v>
+      </c>
+      <c r="CP41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE42">
+        <v>-500</v>
+      </c>
+      <c r="CF42">
+        <v>500</v>
+      </c>
+      <c r="CG42">
+        <v>-5.12</v>
+      </c>
+      <c r="CH42">
+        <v>5.12</v>
+      </c>
+      <c r="CI42">
+        <v>-32</v>
+      </c>
+      <c r="CJ42">
+        <v>32</v>
+      </c>
+      <c r="CK42">
+        <v>-600</v>
+      </c>
+      <c r="CL42">
+        <v>600</v>
+      </c>
+      <c r="CM42">
+        <v>-50</v>
+      </c>
+      <c r="CN42">
+        <v>50</v>
+      </c>
+      <c r="CO42">
+        <v>-50</v>
+      </c>
+      <c r="CP42">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE43">
+        <v>-500</v>
+      </c>
+      <c r="CF43">
+        <v>500</v>
+      </c>
+      <c r="CG43">
+        <v>-5.12</v>
+      </c>
+      <c r="CH43">
+        <v>5.12</v>
+      </c>
+      <c r="CI43">
+        <v>-32</v>
+      </c>
+      <c r="CJ43">
+        <v>32</v>
+      </c>
+      <c r="CK43">
+        <v>-600</v>
+      </c>
+      <c r="CL43">
+        <v>600</v>
+      </c>
+      <c r="CM43">
+        <v>-50</v>
+      </c>
+      <c r="CN43">
+        <v>50</v>
+      </c>
+      <c r="CO43">
+        <v>-50</v>
+      </c>
+      <c r="CP43">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE44">
+        <v>-500</v>
+      </c>
+      <c r="CF44">
+        <v>500</v>
+      </c>
+      <c r="CG44">
+        <v>-5.12</v>
+      </c>
+      <c r="CH44">
+        <v>5.12</v>
+      </c>
+      <c r="CI44">
+        <v>-32</v>
+      </c>
+      <c r="CJ44">
+        <v>32</v>
+      </c>
+      <c r="CK44">
+        <v>-600</v>
+      </c>
+      <c r="CL44">
+        <v>600</v>
+      </c>
+      <c r="CM44">
+        <v>-50</v>
+      </c>
+      <c r="CN44">
+        <v>50</v>
+      </c>
+      <c r="CO44">
+        <v>-50</v>
+      </c>
+      <c r="CP44">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="45" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE45">
+        <v>-500</v>
+      </c>
+      <c r="CF45">
+        <v>500</v>
+      </c>
+      <c r="CG45">
+        <v>-5.12</v>
+      </c>
+      <c r="CH45">
+        <v>5.12</v>
+      </c>
+      <c r="CI45">
+        <v>-32</v>
+      </c>
+      <c r="CJ45">
+        <v>32</v>
+      </c>
+      <c r="CK45">
+        <v>-600</v>
+      </c>
+      <c r="CL45">
+        <v>600</v>
+      </c>
+      <c r="CM45">
+        <v>-50</v>
+      </c>
+      <c r="CN45">
+        <v>50</v>
+      </c>
+      <c r="CO45">
+        <v>-50</v>
+      </c>
+      <c r="CP45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE46">
+        <v>-500</v>
+      </c>
+      <c r="CF46">
+        <v>500</v>
+      </c>
+      <c r="CG46">
+        <v>-5.12</v>
+      </c>
+      <c r="CH46">
+        <v>5.12</v>
+      </c>
+      <c r="CI46">
+        <v>-32</v>
+      </c>
+      <c r="CJ46">
+        <v>32</v>
+      </c>
+      <c r="CK46">
+        <v>-600</v>
+      </c>
+      <c r="CL46">
+        <v>600</v>
+      </c>
+      <c r="CM46">
+        <v>-50</v>
+      </c>
+      <c r="CN46">
+        <v>50</v>
+      </c>
+      <c r="CO46">
+        <v>-50</v>
+      </c>
+      <c r="CP46">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="47" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE47">
+        <v>-500</v>
+      </c>
+      <c r="CF47">
+        <v>500</v>
+      </c>
+      <c r="CG47">
+        <v>-5.12</v>
+      </c>
+      <c r="CH47">
+        <v>5.12</v>
+      </c>
+      <c r="CI47">
+        <v>-32</v>
+      </c>
+      <c r="CJ47">
+        <v>32</v>
+      </c>
+      <c r="CK47">
+        <v>-600</v>
+      </c>
+      <c r="CL47">
+        <v>600</v>
+      </c>
+      <c r="CM47">
+        <v>-50</v>
+      </c>
+      <c r="CN47">
+        <v>50</v>
+      </c>
+      <c r="CO47">
+        <v>-50</v>
+      </c>
+      <c r="CP47">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="48" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE48">
+        <v>-500</v>
+      </c>
+      <c r="CF48">
+        <v>500</v>
+      </c>
+      <c r="CG48">
+        <v>-5.12</v>
+      </c>
+      <c r="CH48">
+        <v>5.12</v>
+      </c>
+      <c r="CI48">
+        <v>-32</v>
+      </c>
+      <c r="CJ48">
+        <v>32</v>
+      </c>
+      <c r="CK48">
+        <v>-600</v>
+      </c>
+      <c r="CL48">
+        <v>600</v>
+      </c>
+      <c r="CM48">
+        <v>-50</v>
+      </c>
+      <c r="CN48">
+        <v>50</v>
+      </c>
+      <c r="CO48">
+        <v>-50</v>
+      </c>
+      <c r="CP48">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE49">
+        <v>-500</v>
+      </c>
+      <c r="CF49">
+        <v>500</v>
+      </c>
+      <c r="CG49">
+        <v>-5.12</v>
+      </c>
+      <c r="CH49">
+        <v>5.12</v>
+      </c>
+      <c r="CI49">
+        <v>-32</v>
+      </c>
+      <c r="CJ49">
+        <v>32</v>
+      </c>
+      <c r="CK49">
+        <v>-600</v>
+      </c>
+      <c r="CL49">
+        <v>600</v>
+      </c>
+      <c r="CM49">
+        <v>-50</v>
+      </c>
+      <c r="CN49">
+        <v>50</v>
+      </c>
+      <c r="CO49">
+        <v>-50</v>
+      </c>
+      <c r="CP49">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE50">
+        <v>-500</v>
+      </c>
+      <c r="CF50">
+        <v>500</v>
+      </c>
+      <c r="CG50">
+        <v>-5.12</v>
+      </c>
+      <c r="CH50">
+        <v>5.12</v>
+      </c>
+      <c r="CI50">
+        <v>-32</v>
+      </c>
+      <c r="CJ50">
+        <v>32</v>
+      </c>
+      <c r="CK50">
+        <v>-600</v>
+      </c>
+      <c r="CL50">
+        <v>600</v>
+      </c>
+      <c r="CM50">
+        <v>-50</v>
+      </c>
+      <c r="CN50">
+        <v>50</v>
+      </c>
+      <c r="CO50">
+        <v>-50</v>
+      </c>
+      <c r="CP50">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE51">
+        <v>-500</v>
+      </c>
+      <c r="CF51">
+        <v>500</v>
+      </c>
+      <c r="CG51">
+        <v>-5.12</v>
+      </c>
+      <c r="CH51">
+        <v>5.12</v>
+      </c>
+      <c r="CI51">
+        <v>-32</v>
+      </c>
+      <c r="CJ51">
+        <v>32</v>
+      </c>
+      <c r="CK51">
+        <v>-600</v>
+      </c>
+      <c r="CL51">
+        <v>600</v>
+      </c>
+      <c r="CM51">
+        <v>-50</v>
+      </c>
+      <c r="CN51">
+        <v>50</v>
+      </c>
+      <c r="CO51">
+        <v>-50</v>
+      </c>
+      <c r="CP51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE52">
+        <v>-500</v>
+      </c>
+      <c r="CF52">
+        <v>500</v>
+      </c>
+      <c r="CG52">
+        <v>-5.12</v>
+      </c>
+      <c r="CH52">
+        <v>5.12</v>
+      </c>
+      <c r="CI52">
+        <v>-32</v>
+      </c>
+      <c r="CJ52">
+        <v>32</v>
+      </c>
+      <c r="CK52">
+        <v>-600</v>
+      </c>
+      <c r="CL52">
+        <v>600</v>
+      </c>
+      <c r="CM52">
+        <v>-50</v>
+      </c>
+      <c r="CN52">
+        <v>50</v>
+      </c>
+      <c r="CO52">
+        <v>-50</v>
+      </c>
+      <c r="CP52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE53">
+        <v>-500</v>
+      </c>
+      <c r="CF53">
+        <v>500</v>
+      </c>
+      <c r="CG53">
+        <v>-5.12</v>
+      </c>
+      <c r="CH53">
+        <v>5.12</v>
+      </c>
+      <c r="CI53">
+        <v>-32</v>
+      </c>
+      <c r="CJ53">
+        <v>32</v>
+      </c>
+      <c r="CK53">
+        <v>-600</v>
+      </c>
+      <c r="CL53">
+        <v>600</v>
+      </c>
+      <c r="CM53">
+        <v>-50</v>
+      </c>
+      <c r="CN53">
+        <v>50</v>
+      </c>
+      <c r="CO53">
+        <v>-50</v>
+      </c>
+      <c r="CP53">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE54">
+        <v>-500</v>
+      </c>
+      <c r="CF54">
+        <v>500</v>
+      </c>
+      <c r="CG54">
+        <v>-5.12</v>
+      </c>
+      <c r="CH54">
+        <v>5.12</v>
+      </c>
+      <c r="CI54">
+        <v>-32</v>
+      </c>
+      <c r="CJ54">
+        <v>32</v>
+      </c>
+      <c r="CK54">
+        <v>-600</v>
+      </c>
+      <c r="CL54">
+        <v>600</v>
+      </c>
+      <c r="CM54">
+        <v>-50</v>
+      </c>
+      <c r="CN54">
+        <v>50</v>
+      </c>
+      <c r="CO54">
+        <v>-50</v>
+      </c>
+      <c r="CP54">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE55">
+        <v>-500</v>
+      </c>
+      <c r="CF55">
+        <v>500</v>
+      </c>
+      <c r="CG55">
+        <v>-5.12</v>
+      </c>
+      <c r="CH55">
+        <v>5.12</v>
+      </c>
+      <c r="CI55">
+        <v>-32</v>
+      </c>
+      <c r="CJ55">
+        <v>32</v>
+      </c>
+      <c r="CK55">
+        <v>-600</v>
+      </c>
+      <c r="CL55">
+        <v>600</v>
+      </c>
+      <c r="CM55">
+        <v>-50</v>
+      </c>
+      <c r="CN55">
+        <v>50</v>
+      </c>
+      <c r="CO55">
+        <v>-50</v>
+      </c>
+      <c r="CP55">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="56" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE56">
+        <v>-500</v>
+      </c>
+      <c r="CF56">
+        <v>500</v>
+      </c>
+      <c r="CG56">
+        <v>-5.12</v>
+      </c>
+      <c r="CH56">
+        <v>5.12</v>
+      </c>
+      <c r="CI56">
+        <v>-32</v>
+      </c>
+      <c r="CJ56">
+        <v>32</v>
+      </c>
+      <c r="CK56">
+        <v>-600</v>
+      </c>
+      <c r="CL56">
+        <v>600</v>
+      </c>
+      <c r="CM56">
+        <v>-50</v>
+      </c>
+      <c r="CN56">
+        <v>50</v>
+      </c>
+      <c r="CO56">
+        <v>-50</v>
+      </c>
+      <c r="CP56">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE57">
+        <v>-500</v>
+      </c>
+      <c r="CF57">
+        <v>500</v>
+      </c>
+      <c r="CG57">
+        <v>-5.12</v>
+      </c>
+      <c r="CH57">
+        <v>5.12</v>
+      </c>
+      <c r="CI57">
+        <v>-32</v>
+      </c>
+      <c r="CJ57">
+        <v>32</v>
+      </c>
+      <c r="CK57">
+        <v>-600</v>
+      </c>
+      <c r="CL57">
+        <v>600</v>
+      </c>
+      <c r="CM57">
+        <v>-50</v>
+      </c>
+      <c r="CN57">
+        <v>50</v>
+      </c>
+      <c r="CO57">
+        <v>-50</v>
+      </c>
+      <c r="CP57">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="58" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE58">
+        <v>-500</v>
+      </c>
+      <c r="CF58">
+        <v>500</v>
+      </c>
+      <c r="CG58">
+        <v>-5.12</v>
+      </c>
+      <c r="CH58">
+        <v>5.12</v>
+      </c>
+      <c r="CI58">
+        <v>-32</v>
+      </c>
+      <c r="CJ58">
+        <v>32</v>
+      </c>
+      <c r="CK58">
+        <v>-600</v>
+      </c>
+      <c r="CL58">
+        <v>600</v>
+      </c>
+      <c r="CM58">
+        <v>-50</v>
+      </c>
+      <c r="CN58">
+        <v>50</v>
+      </c>
+      <c r="CO58">
+        <v>-50</v>
+      </c>
+      <c r="CP58">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="59" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE59">
+        <v>-500</v>
+      </c>
+      <c r="CF59">
+        <v>500</v>
+      </c>
+      <c r="CG59">
+        <v>-5.12</v>
+      </c>
+      <c r="CH59">
+        <v>5.12</v>
+      </c>
+      <c r="CI59">
+        <v>-32</v>
+      </c>
+      <c r="CJ59">
+        <v>32</v>
+      </c>
+      <c r="CK59">
+        <v>-600</v>
+      </c>
+      <c r="CL59">
+        <v>600</v>
+      </c>
+      <c r="CM59">
+        <v>-50</v>
+      </c>
+      <c r="CN59">
+        <v>50</v>
+      </c>
+      <c r="CO59">
+        <v>-50</v>
+      </c>
+      <c r="CP59">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="60" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE60">
+        <v>-500</v>
+      </c>
+      <c r="CF60">
+        <v>500</v>
+      </c>
+      <c r="CG60">
+        <v>-5.12</v>
+      </c>
+      <c r="CH60">
+        <v>5.12</v>
+      </c>
+      <c r="CI60">
+        <v>-32</v>
+      </c>
+      <c r="CJ60">
+        <v>32</v>
+      </c>
+      <c r="CK60">
+        <v>-600</v>
+      </c>
+      <c r="CL60">
+        <v>600</v>
+      </c>
+      <c r="CM60">
+        <v>-50</v>
+      </c>
+      <c r="CN60">
+        <v>50</v>
+      </c>
+      <c r="CO60">
+        <v>-50</v>
+      </c>
+      <c r="CP60">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE61">
+        <v>-500</v>
+      </c>
+      <c r="CF61">
+        <v>500</v>
+      </c>
+      <c r="CG61">
+        <v>-5.12</v>
+      </c>
+      <c r="CH61">
+        <v>5.12</v>
+      </c>
+      <c r="CI61">
+        <v>-32</v>
+      </c>
+      <c r="CJ61">
+        <v>32</v>
+      </c>
+      <c r="CK61">
+        <v>-600</v>
+      </c>
+      <c r="CL61">
+        <v>600</v>
+      </c>
+      <c r="CM61">
+        <v>-50</v>
+      </c>
+      <c r="CN61">
+        <v>50</v>
+      </c>
+      <c r="CO61">
+        <v>-50</v>
+      </c>
+      <c r="CP61">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="62" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE62">
+        <v>-500</v>
+      </c>
+      <c r="CF62">
+        <v>500</v>
+      </c>
+      <c r="CG62">
+        <v>-5.12</v>
+      </c>
+      <c r="CH62">
+        <v>5.12</v>
+      </c>
+      <c r="CI62">
+        <v>-32</v>
+      </c>
+      <c r="CJ62">
+        <v>32</v>
+      </c>
+      <c r="CK62">
+        <v>-600</v>
+      </c>
+      <c r="CL62">
+        <v>600</v>
+      </c>
+      <c r="CM62">
+        <v>-50</v>
+      </c>
+      <c r="CN62">
+        <v>50</v>
+      </c>
+      <c r="CO62">
+        <v>-50</v>
+      </c>
+      <c r="CP62">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE63">
+        <v>-500</v>
+      </c>
+      <c r="CF63">
+        <v>500</v>
+      </c>
+      <c r="CG63">
+        <v>-5.12</v>
+      </c>
+      <c r="CH63">
+        <v>5.12</v>
+      </c>
+      <c r="CI63">
+        <v>-32</v>
+      </c>
+      <c r="CJ63">
+        <v>32</v>
+      </c>
+      <c r="CK63">
+        <v>-600</v>
+      </c>
+      <c r="CL63">
+        <v>600</v>
+      </c>
+      <c r="CM63">
+        <v>-50</v>
+      </c>
+      <c r="CN63">
+        <v>50</v>
+      </c>
+      <c r="CO63">
+        <v>-50</v>
+      </c>
+      <c r="CP63">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="64" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE64">
+        <v>-500</v>
+      </c>
+      <c r="CF64">
+        <v>500</v>
+      </c>
+      <c r="CG64">
+        <v>-5.12</v>
+      </c>
+      <c r="CH64">
+        <v>5.12</v>
+      </c>
+      <c r="CI64">
+        <v>-32</v>
+      </c>
+      <c r="CJ64">
+        <v>32</v>
+      </c>
+      <c r="CK64">
+        <v>-600</v>
+      </c>
+      <c r="CL64">
+        <v>600</v>
+      </c>
+      <c r="CM64">
+        <v>-50</v>
+      </c>
+      <c r="CN64">
+        <v>50</v>
+      </c>
+      <c r="CO64">
+        <v>-50</v>
+      </c>
+      <c r="CP64">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE65">
+        <v>-500</v>
+      </c>
+      <c r="CF65">
+        <v>500</v>
+      </c>
+      <c r="CG65">
+        <v>-5.12</v>
+      </c>
+      <c r="CH65">
+        <v>5.12</v>
+      </c>
+      <c r="CI65">
+        <v>-32</v>
+      </c>
+      <c r="CJ65">
+        <v>32</v>
+      </c>
+      <c r="CK65">
+        <v>-600</v>
+      </c>
+      <c r="CL65">
+        <v>600</v>
+      </c>
+      <c r="CM65">
+        <v>-50</v>
+      </c>
+      <c r="CN65">
+        <v>50</v>
+      </c>
+      <c r="CO65">
+        <v>-50</v>
+      </c>
+      <c r="CP65">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="66" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE66">
+        <v>-500</v>
+      </c>
+      <c r="CF66">
+        <v>500</v>
+      </c>
+      <c r="CG66">
+        <v>-5.12</v>
+      </c>
+      <c r="CH66">
+        <v>5.12</v>
+      </c>
+      <c r="CI66">
+        <v>-32</v>
+      </c>
+      <c r="CJ66">
+        <v>32</v>
+      </c>
+      <c r="CK66">
+        <v>-600</v>
+      </c>
+      <c r="CL66">
+        <v>600</v>
+      </c>
+      <c r="CM66">
+        <v>-50</v>
+      </c>
+      <c r="CN66">
+        <v>50</v>
+      </c>
+      <c r="CO66">
+        <v>-50</v>
+      </c>
+      <c r="CP66">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="67" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE67">
+        <v>-500</v>
+      </c>
+      <c r="CF67">
+        <v>500</v>
+      </c>
+      <c r="CG67">
+        <v>-5.12</v>
+      </c>
+      <c r="CH67">
+        <v>5.12</v>
+      </c>
+      <c r="CI67">
+        <v>-32</v>
+      </c>
+      <c r="CJ67">
+        <v>32</v>
+      </c>
+      <c r="CK67">
+        <v>-600</v>
+      </c>
+      <c r="CL67">
+        <v>600</v>
+      </c>
+      <c r="CM67">
+        <v>-50</v>
+      </c>
+      <c r="CN67">
+        <v>50</v>
+      </c>
+      <c r="CO67">
+        <v>-50</v>
+      </c>
+      <c r="CP67">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE68">
+        <v>-500</v>
+      </c>
+      <c r="CF68">
+        <v>500</v>
+      </c>
+      <c r="CG68">
+        <v>-5.12</v>
+      </c>
+      <c r="CH68">
+        <v>5.12</v>
+      </c>
+      <c r="CI68">
+        <v>-32</v>
+      </c>
+      <c r="CJ68">
+        <v>32</v>
+      </c>
+      <c r="CK68">
+        <v>-600</v>
+      </c>
+      <c r="CL68">
+        <v>600</v>
+      </c>
+      <c r="CM68">
+        <v>-50</v>
+      </c>
+      <c r="CN68">
+        <v>50</v>
+      </c>
+      <c r="CO68">
+        <v>-50</v>
+      </c>
+      <c r="CP68">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE69">
+        <v>-500</v>
+      </c>
+      <c r="CF69">
+        <v>500</v>
+      </c>
+      <c r="CG69">
+        <v>-5.12</v>
+      </c>
+      <c r="CH69">
+        <v>5.12</v>
+      </c>
+      <c r="CI69">
+        <v>-32</v>
+      </c>
+      <c r="CJ69">
+        <v>32</v>
+      </c>
+      <c r="CK69">
+        <v>-600</v>
+      </c>
+      <c r="CL69">
+        <v>600</v>
+      </c>
+      <c r="CM69">
+        <v>-50</v>
+      </c>
+      <c r="CN69">
+        <v>50</v>
+      </c>
+      <c r="CO69">
+        <v>-50</v>
+      </c>
+      <c r="CP69">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE70">
+        <v>-500</v>
+      </c>
+      <c r="CF70">
+        <v>500</v>
+      </c>
+      <c r="CG70">
+        <v>-5.12</v>
+      </c>
+      <c r="CH70">
+        <v>5.12</v>
+      </c>
+      <c r="CI70">
+        <v>-32</v>
+      </c>
+      <c r="CJ70">
+        <v>32</v>
+      </c>
+      <c r="CK70">
+        <v>-600</v>
+      </c>
+      <c r="CL70">
+        <v>600</v>
+      </c>
+      <c r="CM70">
+        <v>-50</v>
+      </c>
+      <c r="CN70">
+        <v>50</v>
+      </c>
+      <c r="CO70">
+        <v>-50</v>
+      </c>
+      <c r="CP70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE71">
+        <v>-500</v>
+      </c>
+      <c r="CF71">
+        <v>500</v>
+      </c>
+      <c r="CG71">
+        <v>-5.12</v>
+      </c>
+      <c r="CH71">
+        <v>5.12</v>
+      </c>
+      <c r="CI71">
+        <v>-32</v>
+      </c>
+      <c r="CJ71">
+        <v>32</v>
+      </c>
+      <c r="CK71">
+        <v>-600</v>
+      </c>
+      <c r="CL71">
+        <v>600</v>
+      </c>
+      <c r="CM71">
+        <v>-50</v>
+      </c>
+      <c r="CN71">
+        <v>50</v>
+      </c>
+      <c r="CO71">
+        <v>-50</v>
+      </c>
+      <c r="CP71">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE72">
+        <v>-500</v>
+      </c>
+      <c r="CF72">
+        <v>500</v>
+      </c>
+      <c r="CG72">
+        <v>-5.12</v>
+      </c>
+      <c r="CH72">
+        <v>5.12</v>
+      </c>
+      <c r="CI72">
+        <v>-32</v>
+      </c>
+      <c r="CJ72">
+        <v>32</v>
+      </c>
+      <c r="CK72">
+        <v>-600</v>
+      </c>
+      <c r="CL72">
+        <v>600</v>
+      </c>
+      <c r="CM72">
+        <v>-50</v>
+      </c>
+      <c r="CN72">
+        <v>50</v>
+      </c>
+      <c r="CO72">
+        <v>-50</v>
+      </c>
+      <c r="CP72">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE73">
+        <v>-500</v>
+      </c>
+      <c r="CF73">
+        <v>500</v>
+      </c>
+      <c r="CG73">
+        <v>-5.12</v>
+      </c>
+      <c r="CH73">
+        <v>5.12</v>
+      </c>
+      <c r="CI73">
+        <v>-32</v>
+      </c>
+      <c r="CJ73">
+        <v>32</v>
+      </c>
+      <c r="CK73">
+        <v>-600</v>
+      </c>
+      <c r="CL73">
+        <v>600</v>
+      </c>
+      <c r="CM73">
+        <v>-50</v>
+      </c>
+      <c r="CN73">
+        <v>50</v>
+      </c>
+      <c r="CO73">
+        <v>-50</v>
+      </c>
+      <c r="CP73">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE74">
+        <v>-500</v>
+      </c>
+      <c r="CF74">
+        <v>500</v>
+      </c>
+      <c r="CG74">
+        <v>-5.12</v>
+      </c>
+      <c r="CH74">
+        <v>5.12</v>
+      </c>
+      <c r="CI74">
+        <v>-32</v>
+      </c>
+      <c r="CJ74">
+        <v>32</v>
+      </c>
+      <c r="CK74">
+        <v>-600</v>
+      </c>
+      <c r="CL74">
+        <v>600</v>
+      </c>
+      <c r="CM74">
+        <v>-50</v>
+      </c>
+      <c r="CN74">
+        <v>50</v>
+      </c>
+      <c r="CO74">
+        <v>-50</v>
+      </c>
+      <c r="CP74">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE75">
+        <v>-500</v>
+      </c>
+      <c r="CF75">
+        <v>500</v>
+      </c>
+      <c r="CG75">
+        <v>-5.12</v>
+      </c>
+      <c r="CH75">
+        <v>5.12</v>
+      </c>
+      <c r="CI75">
+        <v>-32</v>
+      </c>
+      <c r="CJ75">
+        <v>32</v>
+      </c>
+      <c r="CK75">
+        <v>-600</v>
+      </c>
+      <c r="CL75">
+        <v>600</v>
+      </c>
+      <c r="CM75">
+        <v>-50</v>
+      </c>
+      <c r="CN75">
+        <v>50</v>
+      </c>
+      <c r="CO75">
+        <v>-50</v>
+      </c>
+      <c r="CP75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE76">
+        <v>-500</v>
+      </c>
+      <c r="CF76">
+        <v>500</v>
+      </c>
+      <c r="CG76">
+        <v>-5.12</v>
+      </c>
+      <c r="CH76">
+        <v>5.12</v>
+      </c>
+      <c r="CI76">
+        <v>-32</v>
+      </c>
+      <c r="CJ76">
+        <v>32</v>
+      </c>
+      <c r="CK76">
+        <v>-600</v>
+      </c>
+      <c r="CL76">
+        <v>600</v>
+      </c>
+      <c r="CM76">
+        <v>-50</v>
+      </c>
+      <c r="CN76">
+        <v>50</v>
+      </c>
+      <c r="CO76">
+        <v>-50</v>
+      </c>
+      <c r="CP76">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="77" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE77">
+        <v>-500</v>
+      </c>
+      <c r="CF77">
+        <v>500</v>
+      </c>
+      <c r="CG77">
+        <v>-5.12</v>
+      </c>
+      <c r="CH77">
+        <v>5.12</v>
+      </c>
+      <c r="CI77">
+        <v>-32</v>
+      </c>
+      <c r="CJ77">
+        <v>32</v>
+      </c>
+      <c r="CK77">
+        <v>-600</v>
+      </c>
+      <c r="CL77">
+        <v>600</v>
+      </c>
+      <c r="CM77">
+        <v>-50</v>
+      </c>
+      <c r="CN77">
+        <v>50</v>
+      </c>
+      <c r="CO77">
+        <v>-50</v>
+      </c>
+      <c r="CP77">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE78">
+        <v>-500</v>
+      </c>
+      <c r="CF78">
+        <v>500</v>
+      </c>
+      <c r="CG78">
+        <v>-5.12</v>
+      </c>
+      <c r="CH78">
+        <v>5.12</v>
+      </c>
+      <c r="CI78">
+        <v>-32</v>
+      </c>
+      <c r="CJ78">
+        <v>32</v>
+      </c>
+      <c r="CK78">
+        <v>-600</v>
+      </c>
+      <c r="CL78">
+        <v>600</v>
+      </c>
+      <c r="CM78">
+        <v>-50</v>
+      </c>
+      <c r="CN78">
+        <v>50</v>
+      </c>
+      <c r="CO78">
+        <v>-50</v>
+      </c>
+      <c r="CP78">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE79">
+        <v>-500</v>
+      </c>
+      <c r="CF79">
+        <v>500</v>
+      </c>
+      <c r="CG79">
+        <v>-5.12</v>
+      </c>
+      <c r="CH79">
+        <v>5.12</v>
+      </c>
+      <c r="CI79">
+        <v>-32</v>
+      </c>
+      <c r="CJ79">
+        <v>32</v>
+      </c>
+      <c r="CK79">
+        <v>-600</v>
+      </c>
+      <c r="CL79">
+        <v>600</v>
+      </c>
+      <c r="CM79">
+        <v>-50</v>
+      </c>
+      <c r="CN79">
+        <v>50</v>
+      </c>
+      <c r="CO79">
+        <v>-50</v>
+      </c>
+      <c r="CP79">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="80" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE80">
+        <v>-500</v>
+      </c>
+      <c r="CF80">
+        <v>500</v>
+      </c>
+      <c r="CG80">
+        <v>-5.12</v>
+      </c>
+      <c r="CH80">
+        <v>5.12</v>
+      </c>
+      <c r="CI80">
+        <v>-32</v>
+      </c>
+      <c r="CJ80">
+        <v>32</v>
+      </c>
+      <c r="CK80">
+        <v>-600</v>
+      </c>
+      <c r="CL80">
+        <v>600</v>
+      </c>
+      <c r="CM80">
+        <v>-50</v>
+      </c>
+      <c r="CN80">
+        <v>50</v>
+      </c>
+      <c r="CO80">
+        <v>-50</v>
+      </c>
+      <c r="CP80">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="81" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE81">
+        <v>-500</v>
+      </c>
+      <c r="CF81">
+        <v>500</v>
+      </c>
+      <c r="CG81">
+        <v>-5.12</v>
+      </c>
+      <c r="CH81">
+        <v>5.12</v>
+      </c>
+      <c r="CI81">
+        <v>-32</v>
+      </c>
+      <c r="CJ81">
+        <v>32</v>
+      </c>
+      <c r="CK81">
+        <v>-600</v>
+      </c>
+      <c r="CL81">
+        <v>600</v>
+      </c>
+      <c r="CM81">
+        <v>-50</v>
+      </c>
+      <c r="CN81">
+        <v>50</v>
+      </c>
+      <c r="CO81">
+        <v>-50</v>
+      </c>
+      <c r="CP81">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE82">
+        <v>-500</v>
+      </c>
+      <c r="CF82">
+        <v>500</v>
+      </c>
+      <c r="CG82">
+        <v>-5.12</v>
+      </c>
+      <c r="CH82">
+        <v>5.12</v>
+      </c>
+      <c r="CI82">
+        <v>-32</v>
+      </c>
+      <c r="CJ82">
+        <v>32</v>
+      </c>
+      <c r="CK82">
+        <v>-600</v>
+      </c>
+      <c r="CL82">
+        <v>600</v>
+      </c>
+      <c r="CM82">
+        <v>-50</v>
+      </c>
+      <c r="CN82">
+        <v>50</v>
+      </c>
+      <c r="CO82">
+        <v>-50</v>
+      </c>
+      <c r="CP82">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="83" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE83">
+        <v>-500</v>
+      </c>
+      <c r="CF83">
+        <v>500</v>
+      </c>
+      <c r="CG83">
+        <v>-5.12</v>
+      </c>
+      <c r="CH83">
+        <v>5.12</v>
+      </c>
+      <c r="CI83">
+        <v>-32</v>
+      </c>
+      <c r="CJ83">
+        <v>32</v>
+      </c>
+      <c r="CK83">
+        <v>-600</v>
+      </c>
+      <c r="CL83">
+        <v>600</v>
+      </c>
+      <c r="CM83">
+        <v>-50</v>
+      </c>
+      <c r="CN83">
+        <v>50</v>
+      </c>
+      <c r="CO83">
+        <v>-50</v>
+      </c>
+      <c r="CP83">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="84" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE84">
+        <v>-500</v>
+      </c>
+      <c r="CF84">
+        <v>500</v>
+      </c>
+      <c r="CG84">
+        <v>-5.12</v>
+      </c>
+      <c r="CH84">
+        <v>5.12</v>
+      </c>
+      <c r="CI84">
+        <v>-32</v>
+      </c>
+      <c r="CJ84">
+        <v>32</v>
+      </c>
+      <c r="CK84">
+        <v>-600</v>
+      </c>
+      <c r="CL84">
+        <v>600</v>
+      </c>
+      <c r="CM84">
+        <v>-50</v>
+      </c>
+      <c r="CN84">
+        <v>50</v>
+      </c>
+      <c r="CO84">
+        <v>-50</v>
+      </c>
+      <c r="CP84">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="85" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE85">
+        <v>-500</v>
+      </c>
+      <c r="CF85">
+        <v>500</v>
+      </c>
+      <c r="CG85">
+        <v>-5.12</v>
+      </c>
+      <c r="CH85">
+        <v>5.12</v>
+      </c>
+      <c r="CI85">
+        <v>-32</v>
+      </c>
+      <c r="CJ85">
+        <v>32</v>
+      </c>
+      <c r="CK85">
+        <v>-600</v>
+      </c>
+      <c r="CL85">
+        <v>600</v>
+      </c>
+      <c r="CM85">
+        <v>-50</v>
+      </c>
+      <c r="CN85">
+        <v>50</v>
+      </c>
+      <c r="CO85">
+        <v>-50</v>
+      </c>
+      <c r="CP85">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="86" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE86">
+        <v>-500</v>
+      </c>
+      <c r="CF86">
+        <v>500</v>
+      </c>
+      <c r="CG86">
+        <v>-5.12</v>
+      </c>
+      <c r="CH86">
+        <v>5.12</v>
+      </c>
+      <c r="CI86">
+        <v>-32</v>
+      </c>
+      <c r="CJ86">
+        <v>32</v>
+      </c>
+      <c r="CK86">
+        <v>-600</v>
+      </c>
+      <c r="CL86">
+        <v>600</v>
+      </c>
+      <c r="CM86">
+        <v>-50</v>
+      </c>
+      <c r="CN86">
+        <v>50</v>
+      </c>
+      <c r="CO86">
+        <v>-50</v>
+      </c>
+      <c r="CP86">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="87" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE87">
+        <v>-500</v>
+      </c>
+      <c r="CF87">
+        <v>500</v>
+      </c>
+      <c r="CG87">
+        <v>-5.12</v>
+      </c>
+      <c r="CH87">
+        <v>5.12</v>
+      </c>
+      <c r="CI87">
+        <v>-32</v>
+      </c>
+      <c r="CJ87">
+        <v>32</v>
+      </c>
+      <c r="CK87">
+        <v>-600</v>
+      </c>
+      <c r="CL87">
+        <v>600</v>
+      </c>
+      <c r="CM87">
+        <v>-50</v>
+      </c>
+      <c r="CN87">
+        <v>50</v>
+      </c>
+      <c r="CO87">
+        <v>-50</v>
+      </c>
+      <c r="CP87">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="88" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE88">
+        <v>-500</v>
+      </c>
+      <c r="CF88">
+        <v>500</v>
+      </c>
+      <c r="CG88">
+        <v>-5.12</v>
+      </c>
+      <c r="CH88">
+        <v>5.12</v>
+      </c>
+      <c r="CI88">
+        <v>-32</v>
+      </c>
+      <c r="CJ88">
+        <v>32</v>
+      </c>
+      <c r="CK88">
+        <v>-600</v>
+      </c>
+      <c r="CL88">
+        <v>600</v>
+      </c>
+      <c r="CM88">
+        <v>-50</v>
+      </c>
+      <c r="CN88">
+        <v>50</v>
+      </c>
+      <c r="CO88">
+        <v>-50</v>
+      </c>
+      <c r="CP88">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="89" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE89">
+        <v>-500</v>
+      </c>
+      <c r="CF89">
+        <v>500</v>
+      </c>
+      <c r="CG89">
+        <v>-5.12</v>
+      </c>
+      <c r="CH89">
+        <v>5.12</v>
+      </c>
+      <c r="CI89">
+        <v>-32</v>
+      </c>
+      <c r="CJ89">
+        <v>32</v>
+      </c>
+      <c r="CK89">
+        <v>-600</v>
+      </c>
+      <c r="CL89">
+        <v>600</v>
+      </c>
+      <c r="CM89">
+        <v>-50</v>
+      </c>
+      <c r="CN89">
+        <v>50</v>
+      </c>
+      <c r="CO89">
+        <v>-50</v>
+      </c>
+      <c r="CP89">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="90" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE90">
+        <v>-500</v>
+      </c>
+      <c r="CF90">
+        <v>500</v>
+      </c>
+      <c r="CG90">
+        <v>-5.12</v>
+      </c>
+      <c r="CH90">
+        <v>5.12</v>
+      </c>
+      <c r="CI90">
+        <v>-32</v>
+      </c>
+      <c r="CJ90">
+        <v>32</v>
+      </c>
+      <c r="CK90">
+        <v>-600</v>
+      </c>
+      <c r="CL90">
+        <v>600</v>
+      </c>
+      <c r="CM90">
+        <v>-50</v>
+      </c>
+      <c r="CN90">
+        <v>50</v>
+      </c>
+      <c r="CO90">
+        <v>-50</v>
+      </c>
+      <c r="CP90">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="91" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE91">
+        <v>-500</v>
+      </c>
+      <c r="CF91">
+        <v>500</v>
+      </c>
+      <c r="CG91">
+        <v>-5.12</v>
+      </c>
+      <c r="CH91">
+        <v>5.12</v>
+      </c>
+      <c r="CI91">
+        <v>-32</v>
+      </c>
+      <c r="CJ91">
+        <v>32</v>
+      </c>
+      <c r="CK91">
+        <v>-600</v>
+      </c>
+      <c r="CL91">
+        <v>600</v>
+      </c>
+      <c r="CM91">
+        <v>-50</v>
+      </c>
+      <c r="CN91">
+        <v>50</v>
+      </c>
+      <c r="CO91">
+        <v>-50</v>
+      </c>
+      <c r="CP91">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE92">
+        <v>-500</v>
+      </c>
+      <c r="CF92">
+        <v>500</v>
+      </c>
+      <c r="CG92">
+        <v>-5.12</v>
+      </c>
+      <c r="CH92">
+        <v>5.12</v>
+      </c>
+      <c r="CI92">
+        <v>-32</v>
+      </c>
+      <c r="CJ92">
+        <v>32</v>
+      </c>
+      <c r="CK92">
+        <v>-600</v>
+      </c>
+      <c r="CL92">
+        <v>600</v>
+      </c>
+      <c r="CM92">
+        <v>-50</v>
+      </c>
+      <c r="CN92">
+        <v>50</v>
+      </c>
+      <c r="CO92">
+        <v>-50</v>
+      </c>
+      <c r="CP92">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="93" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE93">
+        <v>-500</v>
+      </c>
+      <c r="CF93">
+        <v>500</v>
+      </c>
+      <c r="CG93">
+        <v>-5.12</v>
+      </c>
+      <c r="CH93">
+        <v>5.12</v>
+      </c>
+      <c r="CI93">
+        <v>-32</v>
+      </c>
+      <c r="CJ93">
+        <v>32</v>
+      </c>
+      <c r="CK93">
+        <v>-600</v>
+      </c>
+      <c r="CL93">
+        <v>600</v>
+      </c>
+      <c r="CM93">
+        <v>-50</v>
+      </c>
+      <c r="CN93">
+        <v>50</v>
+      </c>
+      <c r="CO93">
+        <v>-50</v>
+      </c>
+      <c r="CP93">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="94" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE94">
+        <v>-500</v>
+      </c>
+      <c r="CF94">
+        <v>500</v>
+      </c>
+      <c r="CG94">
+        <v>-5.12</v>
+      </c>
+      <c r="CH94">
+        <v>5.12</v>
+      </c>
+      <c r="CI94">
+        <v>-32</v>
+      </c>
+      <c r="CJ94">
+        <v>32</v>
+      </c>
+      <c r="CK94">
+        <v>-600</v>
+      </c>
+      <c r="CL94">
+        <v>600</v>
+      </c>
+      <c r="CM94">
+        <v>-50</v>
+      </c>
+      <c r="CN94">
+        <v>50</v>
+      </c>
+      <c r="CO94">
+        <v>-50</v>
+      </c>
+      <c r="CP94">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE95">
+        <v>-500</v>
+      </c>
+      <c r="CF95">
+        <v>500</v>
+      </c>
+      <c r="CG95">
+        <v>-5.12</v>
+      </c>
+      <c r="CH95">
+        <v>5.12</v>
+      </c>
+      <c r="CI95">
+        <v>-32</v>
+      </c>
+      <c r="CJ95">
+        <v>32</v>
+      </c>
+      <c r="CK95">
+        <v>-600</v>
+      </c>
+      <c r="CL95">
+        <v>600</v>
+      </c>
+      <c r="CM95">
+        <v>-50</v>
+      </c>
+      <c r="CN95">
+        <v>50</v>
+      </c>
+      <c r="CO95">
+        <v>-50</v>
+      </c>
+      <c r="CP95">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE96">
+        <v>-500</v>
+      </c>
+      <c r="CF96">
+        <v>500</v>
+      </c>
+      <c r="CG96">
+        <v>-5.12</v>
+      </c>
+      <c r="CH96">
+        <v>5.12</v>
+      </c>
+      <c r="CI96">
+        <v>-32</v>
+      </c>
+      <c r="CJ96">
+        <v>32</v>
+      </c>
+      <c r="CK96">
+        <v>-600</v>
+      </c>
+      <c r="CL96">
+        <v>600</v>
+      </c>
+      <c r="CM96">
+        <v>-50</v>
+      </c>
+      <c r="CN96">
+        <v>50</v>
+      </c>
+      <c r="CO96">
+        <v>-50</v>
+      </c>
+      <c r="CP96">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE97">
+        <v>-500</v>
+      </c>
+      <c r="CF97">
+        <v>500</v>
+      </c>
+      <c r="CG97">
+        <v>-5.12</v>
+      </c>
+      <c r="CH97">
+        <v>5.12</v>
+      </c>
+      <c r="CI97">
+        <v>-32</v>
+      </c>
+      <c r="CJ97">
+        <v>32</v>
+      </c>
+      <c r="CK97">
+        <v>-600</v>
+      </c>
+      <c r="CL97">
+        <v>600</v>
+      </c>
+      <c r="CM97">
+        <v>-50</v>
+      </c>
+      <c r="CN97">
+        <v>50</v>
+      </c>
+      <c r="CO97">
+        <v>-50</v>
+      </c>
+      <c r="CP97">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="98" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE98">
+        <v>-500</v>
+      </c>
+      <c r="CF98">
+        <v>500</v>
+      </c>
+      <c r="CG98">
+        <v>-5.12</v>
+      </c>
+      <c r="CH98">
+        <v>5.12</v>
+      </c>
+      <c r="CI98">
+        <v>-32</v>
+      </c>
+      <c r="CJ98">
+        <v>32</v>
+      </c>
+      <c r="CK98">
+        <v>-600</v>
+      </c>
+      <c r="CL98">
+        <v>600</v>
+      </c>
+      <c r="CM98">
+        <v>-50</v>
+      </c>
+      <c r="CN98">
+        <v>50</v>
+      </c>
+      <c r="CO98">
+        <v>-50</v>
+      </c>
+      <c r="CP98">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="99" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE99">
+        <v>-500</v>
+      </c>
+      <c r="CF99">
+        <v>500</v>
+      </c>
+      <c r="CG99">
+        <v>-5.12</v>
+      </c>
+      <c r="CH99">
+        <v>5.12</v>
+      </c>
+      <c r="CI99">
+        <v>-32</v>
+      </c>
+      <c r="CJ99">
+        <v>32</v>
+      </c>
+      <c r="CK99">
+        <v>-600</v>
+      </c>
+      <c r="CL99">
+        <v>600</v>
+      </c>
+      <c r="CM99">
+        <v>-50</v>
+      </c>
+      <c r="CN99">
+        <v>50</v>
+      </c>
+      <c r="CO99">
+        <v>-50</v>
+      </c>
+      <c r="CP99">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="100" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE100">
+        <v>-500</v>
+      </c>
+      <c r="CF100">
+        <v>500</v>
+      </c>
+      <c r="CG100">
+        <v>-5.12</v>
+      </c>
+      <c r="CH100">
+        <v>5.12</v>
+      </c>
+      <c r="CI100">
+        <v>-32</v>
+      </c>
+      <c r="CJ100">
+        <v>32</v>
+      </c>
+      <c r="CK100">
+        <v>-600</v>
+      </c>
+      <c r="CL100">
+        <v>600</v>
+      </c>
+      <c r="CM100">
+        <v>-50</v>
+      </c>
+      <c r="CN100">
+        <v>50</v>
+      </c>
+      <c r="CO100">
+        <v>-50</v>
+      </c>
+      <c r="CP100">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="101" spans="83:94" x14ac:dyDescent="0.25">
+      <c r="CE101">
+        <v>-500</v>
+      </c>
+      <c r="CF101">
+        <v>500</v>
+      </c>
+      <c r="CG101">
+        <v>-5.12</v>
+      </c>
+      <c r="CH101">
+        <v>5.12</v>
+      </c>
+      <c r="CI101">
+        <v>-32</v>
+      </c>
+      <c r="CJ101">
+        <v>32</v>
+      </c>
+      <c r="CK101">
+        <v>-600</v>
+      </c>
+      <c r="CL101">
+        <v>600</v>
+      </c>
+      <c r="CM101">
+        <v>-50</v>
+      </c>
+      <c r="CN101">
+        <v>50</v>
+      </c>
+      <c r="CO101">
+        <v>-50</v>
+      </c>
+      <c r="CP101">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>